<commit_message>
Rendu à changer en model uml
</commit_message>
<xml_diff>
--- a/Ressources/ModelBD/EtapeTransformationModelBD.xlsx
+++ b/Ressources/ModelBD/EtapeTransformationModelBD.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="69">
   <si>
     <t>Créer le modèle conceptuel de données</t>
   </si>
@@ -541,6 +541,9 @@
       </rPr>
       <t>Générer les noms physiques (Outils / Générer / Noms physiques) (longueur de 20 et nombre case au moins 20)(minuscule)(status: complet)</t>
     </r>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -1194,7 +1197,7 @@
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="K13" sqref="K13"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1235,7 +1238,9 @@
       <c r="B4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="17"/>
+      <c r="C4" s="17" t="s">
+        <v>58</v>
+      </c>
       <c r="E4" s="28"/>
       <c r="F4" s="28"/>
       <c r="G4" s="28"/>
@@ -1248,7 +1253,9 @@
       <c r="B5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="17"/>
+      <c r="C5" s="17" t="s">
+        <v>58</v>
+      </c>
       <c r="E5" s="28"/>
       <c r="F5" s="28"/>
       <c r="G5" s="28"/>
@@ -1261,7 +1268,9 @@
       <c r="B6" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="18"/>
+      <c r="C6" s="18" t="s">
+        <v>58</v>
+      </c>
       <c r="E6" s="28"/>
       <c r="F6" s="28"/>
       <c r="G6" s="28"/>
@@ -1292,7 +1301,9 @@
       <c r="B9" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="23"/>
+      <c r="C9" s="23" t="s">
+        <v>58</v>
+      </c>
       <c r="E9" s="29"/>
       <c r="F9" s="29"/>
       <c r="G9" s="29"/>
@@ -1305,7 +1316,9 @@
       <c r="B10" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="17"/>
+      <c r="C10" s="17" t="s">
+        <v>58</v>
+      </c>
       <c r="E10" s="29"/>
       <c r="F10" s="29"/>
       <c r="G10" s="29"/>
@@ -1316,7 +1329,9 @@
       <c r="B11" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="C11" s="17"/>
+      <c r="C11" s="17" t="s">
+        <v>58</v>
+      </c>
       <c r="E11" s="29"/>
       <c r="F11" s="29"/>
       <c r="G11" s="29"/>
@@ -1329,7 +1344,9 @@
       <c r="B12" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="17"/>
+      <c r="C12" s="17" t="s">
+        <v>68</v>
+      </c>
       <c r="E12" s="29"/>
       <c r="F12" s="29"/>
       <c r="G12" s="29"/>

</xml_diff>

<commit_message>
Début de transformation du model, maintenant en model relationnel de BD
</commit_message>
<xml_diff>
--- a/Ressources/ModelBD/EtapeTransformationModelBD.xlsx
+++ b/Ressources/ModelBD/EtapeTransformationModelBD.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="69">
   <si>
     <t>Créer le modèle conceptuel de données</t>
   </si>
@@ -1195,9 +1195,9 @@
   <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomLeft" activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1359,7 +1359,9 @@
       <c r="B13" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="17"/>
+      <c r="C13" s="17" t="s">
+        <v>58</v>
+      </c>
       <c r="E13" s="29"/>
       <c r="F13" s="29"/>
       <c r="G13" s="29"/>
@@ -1372,7 +1374,9 @@
       <c r="B14" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="17"/>
+      <c r="C14" s="17" t="s">
+        <v>58</v>
+      </c>
       <c r="E14" s="29"/>
       <c r="F14" s="29"/>
       <c r="G14" s="29"/>
@@ -1405,7 +1409,9 @@
       <c r="B17" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="17"/>
+      <c r="C17" s="17" t="s">
+        <v>58</v>
+      </c>
       <c r="E17" s="29"/>
       <c r="F17" s="29"/>
       <c r="G17" s="29"/>
@@ -1418,7 +1424,9 @@
       <c r="B18" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="17"/>
+      <c r="C18" s="17" t="s">
+        <v>58</v>
+      </c>
       <c r="E18" s="29"/>
       <c r="F18" s="29"/>
       <c r="G18" s="29"/>
@@ -1429,7 +1437,9 @@
       <c r="B19" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="C19" s="17"/>
+      <c r="C19" s="17" t="s">
+        <v>58</v>
+      </c>
       <c r="E19" s="29"/>
       <c r="F19" s="29"/>
       <c r="G19" s="29"/>
@@ -1442,7 +1452,9 @@
       <c r="B20" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="17"/>
+      <c r="C20" s="17" t="s">
+        <v>58</v>
+      </c>
       <c r="E20" s="29"/>
       <c r="F20" s="29"/>
       <c r="G20" s="29"/>
@@ -1455,7 +1467,9 @@
       <c r="B21" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="C21" s="17"/>
+      <c r="C21" s="17" t="s">
+        <v>58</v>
+      </c>
       <c r="E21" s="29"/>
       <c r="F21" s="29"/>
       <c r="G21" s="29"/>

</xml_diff>

<commit_message>
Oh shit le model est rendu trop gros!!!
</commit_message>
<xml_diff>
--- a/Ressources/ModelBD/EtapeTransformationModelBD.xlsx
+++ b/Ressources/ModelBD/EtapeTransformationModelBD.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="69">
   <si>
     <t>Créer le modèle conceptuel de données</t>
   </si>
@@ -1194,10 +1194,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="I23" sqref="I23"/>
+      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1482,7 +1482,9 @@
       <c r="B22" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="17"/>
+      <c r="C22" s="17" t="s">
+        <v>58</v>
+      </c>
       <c r="E22" s="29"/>
       <c r="F22" s="29"/>
       <c r="G22" s="29"/>
@@ -1495,7 +1497,9 @@
       <c r="B23" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="17"/>
+      <c r="C23" s="17" t="s">
+        <v>58</v>
+      </c>
       <c r="E23" s="29"/>
       <c r="F23" s="29"/>
       <c r="G23" s="29"/>
@@ -1508,7 +1512,9 @@
       <c r="B24" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="17"/>
+      <c r="C24" s="17" t="s">
+        <v>58</v>
+      </c>
       <c r="E24" s="29"/>
       <c r="F24" s="29"/>
       <c r="G24" s="29"/>

</xml_diff>

<commit_message>
On a finalement le sql de la BD !!!
</commit_message>
<xml_diff>
--- a/Ressources/ModelBD/EtapeTransformationModelBD.xlsx
+++ b/Ressources/ModelBD/EtapeTransformationModelBD.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="69">
   <si>
     <t>Créer le modèle conceptuel de données</t>
   </si>
@@ -1195,9 +1195,9 @@
   <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
+      <selection pane="bottomLeft" activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1525,7 +1525,9 @@
       <c r="B25" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="17"/>
+      <c r="C25" s="17" t="s">
+        <v>58</v>
+      </c>
       <c r="E25" s="29"/>
       <c r="F25" s="29"/>
       <c r="G25" s="29"/>
@@ -1536,7 +1538,9 @@
       <c r="B26" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="C26" s="17"/>
+      <c r="C26" s="17" t="s">
+        <v>58</v>
+      </c>
       <c r="E26" s="29"/>
       <c r="F26" s="29"/>
       <c r="G26" s="29"/>
@@ -1549,7 +1553,9 @@
       <c r="B27" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C27" s="17"/>
+      <c r="C27" s="17" t="s">
+        <v>58</v>
+      </c>
       <c r="E27" s="29"/>
       <c r="F27" s="29"/>
       <c r="G27" s="29"/>
@@ -1582,7 +1588,9 @@
       <c r="B30" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="C30" s="17"/>
+      <c r="C30" s="17" t="s">
+        <v>58</v>
+      </c>
       <c r="E30" s="29"/>
       <c r="F30" s="29"/>
       <c r="G30" s="29"/>
@@ -1595,7 +1603,9 @@
       <c r="B31" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C31" s="17"/>
+      <c r="C31" s="17" t="s">
+        <v>58</v>
+      </c>
       <c r="E31" s="29"/>
       <c r="F31" s="29"/>
       <c r="G31" s="29"/>
@@ -1608,7 +1618,9 @@
       <c r="B32" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C32" s="17"/>
+      <c r="C32" s="17" t="s">
+        <v>58</v>
+      </c>
       <c r="E32" s="29"/>
       <c r="F32" s="29"/>
       <c r="G32" s="29"/>

</xml_diff>

<commit_message>
Réglage de bogue sur la BD
</commit_message>
<xml_diff>
--- a/Ressources/ModelBD/EtapeTransformationModelBD.xlsx
+++ b/Ressources/ModelBD/EtapeTransformationModelBD.xlsx
@@ -1195,9 +1195,9 @@
   <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="C33" sqref="C33"/>
+      <selection pane="bottomLeft" activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>